<commit_message>
some more bug fixes
</commit_message>
<xml_diff>
--- a/data/original/kf23_dataark_-_landbrug.xlsx
+++ b/data/original/kf23_dataark_-_landbrug.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{B0DDC718-100D-4010-9A34-67F04E8643A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7218CB44-231D-4290-B058-84B126613B05}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{B0DDC718-100D-4010-9A34-67F04E8643A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2550B5C-1A06-4FFF-9618-0D9CCBFA0378}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-25260" yWindow="1290" windowWidth="21600" windowHeight="11295" tabRatio="846" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="846" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Velkommen" sheetId="17" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="354">
   <si>
     <t xml:space="preserve">Tabellerne i fanerne i denne excel-mappe giver en oversigt over de væsentligste beregningsforudsætninger DCE anvender til at beregne drivhusgasudledninger fra landbruget til Klimafremskrivning 2022 </t>
   </si>
@@ -1086,6 +1086,63 @@
   <si>
     <t>svin% i alt</t>
   </si>
+  <si>
+    <t>ab_lager</t>
+  </si>
+  <si>
+    <t>ab_stald</t>
+  </si>
+  <si>
+    <t>model_gruppe</t>
+  </si>
+  <si>
+    <t>ab_dyr</t>
+  </si>
+  <si>
+    <t>toklimastald_smågrise</t>
+  </si>
+  <si>
+    <t>spalter_smågrise</t>
+  </si>
+  <si>
+    <t>spalter_33_67_slagtesvin</t>
+  </si>
+  <si>
+    <t>spalter_50_75_slagtesvin</t>
+  </si>
+  <si>
+    <t>spalter_25_50_slagtesvin</t>
+  </si>
+  <si>
+    <t>løs_individuel_søer</t>
+  </si>
+  <si>
+    <t>farestald_delvis_spalte</t>
+  </si>
+  <si>
+    <t>farestald_fuldspalte</t>
+  </si>
+  <si>
+    <t>kvæg_ringkanal</t>
+  </si>
+  <si>
+    <t>kvæg_fast_skrab</t>
+  </si>
+  <si>
+    <t>kvæg_spalter_skrab</t>
+  </si>
+  <si>
+    <t>kvæg_hæld_fast_skrab</t>
+  </si>
+  <si>
+    <t>kvæg_andre_hyppig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">svin_abstald </t>
+  </si>
+  <si>
+    <t>kvæg_abstald</t>
+  </si>
 </sst>
 </file>
 
@@ -1098,7 +1155,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1256,6 +1313,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1353,7 +1416,7 @@
     <xf numFmtId="9" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1589,6 +1652,7 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma" xfId="7" builtinId="3"/>
@@ -2416,10 +2480,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:AZ24"/>
+  <dimension ref="A1:BT34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AG23" sqref="AG23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL35" sqref="AL35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3032,7 +3096,247 @@
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
     </row>
-    <row r="23" spans="22:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AR13" t="s">
+        <v>337</v>
+      </c>
+      <c r="AS13" t="s">
+        <v>338</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>336</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AK14" t="s">
+        <v>335</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>336</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>339</v>
+      </c>
+      <c r="AS14">
+        <v>0.09</v>
+      </c>
+      <c r="AT14">
+        <v>0.13</v>
+      </c>
+      <c r="AU14">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AI15" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="AJ15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK15" s="13">
+        <v>2021</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>340</v>
+      </c>
+      <c r="AS15">
+        <v>0.09</v>
+      </c>
+      <c r="AT15">
+        <v>0.12</v>
+      </c>
+      <c r="AU15">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AI16" t="s">
+        <v>235</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK16" s="39">
+        <v>16369820.093135342</v>
+      </c>
+      <c r="AL16">
+        <f>AK16*AT22/AU22</f>
+        <v>17761106.791828584</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>341</v>
+      </c>
+      <c r="AS16">
+        <v>0.5</v>
+      </c>
+      <c r="AT16">
+        <v>0.59</v>
+      </c>
+      <c r="AU16">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="22:72" x14ac:dyDescent="0.25">
+      <c r="AJ17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK17" s="39">
+        <v>2279437.1970389588</v>
+      </c>
+      <c r="AL17">
+        <f>AK17*AT23/AU23</f>
+        <v>2473168.7490476952</v>
+      </c>
+      <c r="AM17" s="39"/>
+      <c r="AN17" s="39"/>
+      <c r="AO17" s="39"/>
+      <c r="AR17" t="s">
+        <v>342</v>
+      </c>
+      <c r="AS17">
+        <v>0.5</v>
+      </c>
+      <c r="AT17">
+        <v>0.6</v>
+      </c>
+      <c r="AU17">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="18" spans="22:72" x14ac:dyDescent="0.25">
+      <c r="AJ18" t="s">
+        <v>89</v>
+      </c>
+      <c r="AK18" s="39">
+        <v>6119516.2642199993</v>
+      </c>
+      <c r="AL18" s="39">
+        <f>AK18*AT19/AU19</f>
+        <v>4179181.8389795115</v>
+      </c>
+      <c r="AM18" s="39"/>
+      <c r="AN18" s="39"/>
+      <c r="AO18" s="39"/>
+      <c r="AR18" t="s">
+        <v>343</v>
+      </c>
+      <c r="AS18">
+        <v>0.5</v>
+      </c>
+      <c r="AT18">
+        <v>0.6</v>
+      </c>
+      <c r="AU18">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="19" spans="22:72" x14ac:dyDescent="0.25">
+      <c r="AJ19" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK19" s="39">
+        <v>3876248.6047300003</v>
+      </c>
+      <c r="AL19" s="39">
+        <f>AK19</f>
+        <v>3876248.6047300003</v>
+      </c>
+      <c r="AM19" s="39"/>
+      <c r="AN19" s="39"/>
+      <c r="AO19" s="39"/>
+      <c r="AR19" t="s">
+        <v>344</v>
+      </c>
+      <c r="AS19">
+        <v>2.82</v>
+      </c>
+      <c r="AT19">
+        <v>2.8</v>
+      </c>
+      <c r="AU19">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="22:72" x14ac:dyDescent="0.25">
+      <c r="AJ20" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK20" s="39">
+        <v>11052477.611959999</v>
+      </c>
+      <c r="AL20" s="39">
+        <f>AK20*(AVERAGE(AT16:AT18)/AVERAGE(AU16:AU18))</f>
+        <v>12137383.389821105</v>
+      </c>
+      <c r="AM20" s="39"/>
+      <c r="AN20" s="39"/>
+      <c r="AO20" s="39"/>
+      <c r="AR20" t="s">
+        <v>345</v>
+      </c>
+      <c r="AS20">
+        <v>1.21</v>
+      </c>
+      <c r="AT20">
+        <v>1.27</v>
+      </c>
+      <c r="AU20">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="21" spans="22:72" x14ac:dyDescent="0.25">
+      <c r="AJ21" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK21" s="39">
+        <v>0</v>
+      </c>
+      <c r="AL21" s="39"/>
+      <c r="AM21" s="39"/>
+      <c r="AN21" s="39"/>
+      <c r="AO21" s="39"/>
+      <c r="AR21" t="s">
+        <v>346</v>
+      </c>
+      <c r="AS21">
+        <v>1.21</v>
+      </c>
+      <c r="AT21">
+        <v>1.27</v>
+      </c>
+      <c r="AU21">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="22" spans="22:72" x14ac:dyDescent="0.25">
+      <c r="AJ22" t="s">
+        <v>171</v>
+      </c>
+      <c r="AK22" s="39">
+        <v>112.6905</v>
+      </c>
+      <c r="AL22" s="39"/>
+      <c r="AM22" s="39"/>
+      <c r="AN22" s="39"/>
+      <c r="AO22" s="39"/>
+      <c r="AR22" t="s">
+        <v>347</v>
+      </c>
+      <c r="AS22">
+        <v>28.06</v>
+      </c>
+      <c r="AT22">
+        <v>36</v>
+      </c>
+      <c r="AU22">
+        <v>33.18</v>
+      </c>
+    </row>
+    <row r="23" spans="22:72" x14ac:dyDescent="0.25">
       <c r="V23" t="s">
         <v>331</v>
       </c>
@@ -3050,8 +3354,30 @@
         <f>AF23/AA23</f>
         <v>0.18669826755206634</v>
       </c>
+      <c r="AJ23" t="s">
+        <v>178</v>
+      </c>
+      <c r="AK23" s="39">
+        <v>0</v>
+      </c>
+      <c r="AL23" s="39"/>
+      <c r="AM23" s="39"/>
+      <c r="AN23" s="39"/>
+      <c r="AO23" s="39"/>
+      <c r="AR23" t="s">
+        <v>348</v>
+      </c>
+      <c r="AS23">
+        <v>28.06</v>
+      </c>
+      <c r="AT23">
+        <v>36</v>
+      </c>
+      <c r="AU23">
+        <v>33.18</v>
+      </c>
     </row>
-    <row r="24" spans="22:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="22:72" x14ac:dyDescent="0.25">
       <c r="V24" t="s">
         <v>332</v>
       </c>
@@ -3068,6 +3394,142 @@
       <c r="AG24">
         <f>AF24/AA24</f>
         <v>0.27993566152232446</v>
+      </c>
+      <c r="AJ24" t="s">
+        <v>236</v>
+      </c>
+      <c r="AK24" s="39">
+        <v>0</v>
+      </c>
+      <c r="AL24" s="39"/>
+      <c r="AM24" s="39"/>
+      <c r="AN24" s="39"/>
+      <c r="AO24" s="39"/>
+      <c r="AR24" t="s">
+        <v>349</v>
+      </c>
+      <c r="AS24">
+        <v>28.06</v>
+      </c>
+      <c r="AT24">
+        <v>36</v>
+      </c>
+      <c r="AU24">
+        <v>33.18</v>
+      </c>
+    </row>
+    <row r="25" spans="22:72" x14ac:dyDescent="0.25">
+      <c r="AJ25" t="s">
+        <v>96</v>
+      </c>
+      <c r="AK25" s="39">
+        <v>0</v>
+      </c>
+      <c r="AL25" s="39"/>
+      <c r="AM25" s="39"/>
+      <c r="AN25" s="39"/>
+      <c r="AO25" s="39"/>
+      <c r="AR25" t="s">
+        <v>350</v>
+      </c>
+      <c r="AS25">
+        <v>28.06</v>
+      </c>
+      <c r="AT25">
+        <v>36</v>
+      </c>
+      <c r="AU25">
+        <v>33.18</v>
+      </c>
+    </row>
+    <row r="26" spans="22:72" x14ac:dyDescent="0.25">
+      <c r="AI26" s="4"/>
+      <c r="AJ26" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AK26" s="44">
+        <v>0</v>
+      </c>
+      <c r="AL26" s="39"/>
+      <c r="AM26" s="39"/>
+      <c r="AN26" s="39"/>
+      <c r="AO26" s="39"/>
+      <c r="AR26" t="s">
+        <v>351</v>
+      </c>
+      <c r="AS26">
+        <v>28.06</v>
+      </c>
+      <c r="AT26">
+        <v>28.3</v>
+      </c>
+      <c r="AU26">
+        <v>33.07</v>
+      </c>
+    </row>
+    <row r="27" spans="22:72" x14ac:dyDescent="0.25">
+      <c r="AM27" s="4"/>
+      <c r="AN27" s="4"/>
+      <c r="AO27" s="44"/>
+      <c r="AP27" s="44"/>
+      <c r="AQ27" s="44"/>
+      <c r="AR27" s="44"/>
+      <c r="AS27" s="44"/>
+      <c r="AT27" s="44"/>
+      <c r="AU27" s="44"/>
+      <c r="AV27" s="44"/>
+      <c r="AW27" s="44"/>
+      <c r="AX27" s="44"/>
+      <c r="AY27" s="44"/>
+      <c r="AZ27" s="44"/>
+      <c r="BA27" s="44"/>
+      <c r="BB27" s="44"/>
+      <c r="BC27" s="44"/>
+      <c r="BD27" s="44"/>
+      <c r="BE27" s="44"/>
+      <c r="BF27" s="44"/>
+      <c r="BG27" s="44"/>
+      <c r="BH27" s="44"/>
+      <c r="BI27" s="44"/>
+      <c r="BJ27" s="44"/>
+      <c r="BK27" s="44"/>
+      <c r="BL27" s="44"/>
+      <c r="BM27" s="44"/>
+      <c r="BN27" s="44"/>
+      <c r="BO27" s="44"/>
+      <c r="BP27" s="44"/>
+      <c r="BQ27" s="44"/>
+      <c r="BR27" s="44"/>
+      <c r="BS27" s="44"/>
+      <c r="BT27" s="44"/>
+    </row>
+    <row r="28" spans="22:72" x14ac:dyDescent="0.25">
+      <c r="AA28" s="127"/>
+    </row>
+    <row r="33" spans="36:38" x14ac:dyDescent="0.25">
+      <c r="AJ33" t="s">
+        <v>352</v>
+      </c>
+      <c r="AK33" s="6">
+        <f>SUM(AL18:AL20)</f>
+        <v>20192813.833530616</v>
+      </c>
+      <c r="AL33">
+        <f>AF23/AK33</f>
+        <v>0.1806755591675609</v>
+      </c>
+    </row>
+    <row r="34" spans="36:38" x14ac:dyDescent="0.25">
+      <c r="AJ34" t="s">
+        <v>353</v>
+      </c>
+      <c r="AK34">
+        <f>SUM(AL16:AL17)</f>
+        <v>20234275.540876281</v>
+      </c>
+      <c r="AL34">
+        <f>AF24/AK34</f>
+        <v>0.29290651189796585</v>
       </c>
     </row>
   </sheetData>
@@ -61039,10 +61501,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:BA34"/>
+  <dimension ref="A1:BA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AH6" sqref="A6:AH17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64755,17 +65217,27 @@
         <v>0.11707947389579378</v>
       </c>
     </row>
-    <row r="33" spans="18:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="18:34" x14ac:dyDescent="0.25">
       <c r="R33" s="6"/>
       <c r="W33" s="39">
         <v>6151515.6510000005</v>
       </c>
       <c r="AB33" s="6"/>
     </row>
-    <row r="34" spans="18:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="18:34" x14ac:dyDescent="0.25">
       <c r="W34">
         <f>4192784*0.4/SUM(AG9:AG11)</f>
         <v>7.5658155570930738E-2</v>
+      </c>
+      <c r="AH34" s="6">
+        <f>SUM(AH7:AH8,AH18:AH19)</f>
+        <v>21747166.21103159</v>
+      </c>
+    </row>
+    <row r="36" spans="18:34" x14ac:dyDescent="0.25">
+      <c r="AH36" s="6">
+        <f>SUM(AH9:AH11,AH20:AH22)</f>
+        <v>21330625.65526</v>
       </c>
     </row>
   </sheetData>
@@ -68348,23 +68820,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="84f42352-3182-481c-87ea-4ab76f0f3ad6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BFA6A795B3264D4F859ECB954B11F065" ma:contentTypeVersion="15" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="02d272c11bd3b8793e1995c8220e0933">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="84f42352-3182-481c-87ea-4ab76f0f3ad6" xmlns:ns4="fce77e05-e53d-40e3-924c-010633414056" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="473fbb321356672efa010ec8c0bf0901" ns3:_="" ns4:_="">
     <xsd:import namespace="84f42352-3182-481c-87ea-4ab76f0f3ad6"/>
@@ -68599,25 +69054,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{312EF916-AB78-462C-8F5E-8D6B1DB04AEA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="84f42352-3182-481c-87ea-4ab76f0f3ad6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE1B9B53-EAB5-437A-8546-AEFE508DD20E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="84f42352-3182-481c-87ea-4ab76f0f3ad6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36010F80-1375-43C3-B6C8-B9B47EE7259A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -68634,4 +69088,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE1B9B53-EAB5-437A-8546-AEFE508DD20E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{312EF916-AB78-462C-8F5E-8D6B1DB04AEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="84f42352-3182-481c-87ea-4ab76f0f3ad6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>